<commit_message>
Test plan: added new tests to be implemented
</commit_message>
<xml_diff>
--- a/SystemDescriptor test plan.xlsx
+++ b/SystemDescriptor test plan.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristi\PycharmProjects\SystemDescriptor\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="3" r:id="rId1"/>
     <sheet name="Overview" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Overview!$A$1:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Overview!$A$1:$E$37</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="115">
   <si>
     <t>Requirements</t>
   </si>
@@ -459,13 +464,7 @@
     </r>
   </si>
   <si>
-    <t>- check that only one mapping (SENDER-RECEIVER-TO-SIGNAL-MAPPING) is present in the produced arxml file</t>
-  </si>
-  <si>
     <t>- check that both mapping (SENDER-RECEIVER-TO-SIGNAL-MAPPING) are present in the produced arxml file</t>
-  </si>
-  <si>
-    <t>- check that only one mapping (SWC-TO-ECU-MAPPING) is present in the produced arxml file</t>
   </si>
   <si>
     <t>- check that only one  mapping (SWC-TO-ECU-MAPPING) is present in the produced arxml file, that will contain all the components from both input mappings</t>
@@ -652,25 +651,23 @@
     <r>
       <rPr>
         <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: provide to the tool two ".dico" files, each one of them having the definition of the same mapping, and each mapping (SENDER-RECEIVER-TO-SIGNAL-MAPPING) having the exactly same data</t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide to the tool two ".dico" files, each one of them having the definition of the same mapping, and each mapping (SWC-TO-ECU-MAPPING) having the exactly same short-name and components, but different ECU-INSTANCE-REF</t>
     </r>
   </si>
   <si>
@@ -683,6 +680,136 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Test 10:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> provide to the tool two ".dico" files, each one of them having the definition of the same composition and each composition (COMPOSITION-SW-COMPONENT-TYPE) having the exactly same short-name but different components (each component having the same short-name but different TYPE-TREF)</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that both compositions are present in the produced output file</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 9:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> provide to the tool two ".dico" files, each one of them having different definitions of compositions (SHORT-NAME and components)</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that the output file does not contain the interface definition</t>
+  </si>
+  <si>
+    <t>- check that the output file does not contain the data-type definition</t>
+  </si>
+  <si>
+    <t>- check that the output arxml file contains the definition of that compu-method and keeps the same package name</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: provide to the tool two ".dico" files, each one of them having the definition of the same compu-method, and compu-method type having the same short name </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide to the tool one arxml file and one dico file each of them having the definition of the same compu-method</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that the output file does not contain the compu-method definition</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide to the tool one arxml file and one dico file each of them having the definition of the same interface</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Test 6</t>
     </r>
     <r>
@@ -693,33 +820,34 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: provide to the tool two ".dico" files, each one of them having the definition of the same mapping, and each mapping (SWC-TO-ECU-MAPPING) having the exactly same short-name and components, but different ECU-INSTANCE-REF</t>
+      <t>: provide to the tool one arxml file and one dico file each of them having the definition of the same data-type</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 3</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: provide to the tool two ".dico" files, each one of them having the definition of the same mapping, and each mapping (SWC-TO-ECU-MAPPING) having the exactly same short-name and components</t>
-    </r>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide to the tool two ".dico" files, each one of them having the definition of the same composition-prototype and each composition-prototype (ROOT-SW-COMPOSITION-PROTOTYPE) having the exactly same SHORT-NAME and SOFTWARE-COMPOSITION-TREF</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that only one composition-prototype (ROOT-SW-COMPOSITION-PROTOTYPE) is present in the produced arxml file</t>
   </si>
   <si>
     <r>
@@ -731,21 +859,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test 10:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> provide to the tool two ".dico" files, each one of them having the definition of the same composition and each composition (COMPOSITION-SW-COMPONENT-TYPE) having the exactly same short-name but different components (each component having the same short-name but different TYPE-TREF)</t>
-    </r>
-  </si>
-  <si>
-    <t>- check that both compositions are present in the produced output file</t>
+      <t>Test 14:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> provide to the tool two ".dico" files, each one of them having the definition of the same composition and each composition (ROOT-SW-COMPOSITION-PROTOTYPE) having the exactly same short-name but different SOFTWARE-COMPOSITION-TREF </t>
+    </r>
   </si>
   <si>
     <r>
@@ -757,25 +882,127 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test 9:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> provide to the tool two ".dico" files, each one of them having different definitions of compositions (SHORT-NAME and components)</t>
-    </r>
+      <t>Test 12:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> provide to the tool two ".dico" files, each one of them having the definition of the same composition and each composition (ROOT-SW-COMPOSITION-PROTOTYPE) having the exactly same short-name but different components-prototype</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that only one  composition (ROOT-SW-COMPOSITION-PROTOTYPE) is present in the produced arxml file, that will contain all the components-prototype</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 13:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> provide to the tool two ".dico" files, each one of them having different definitions of compositions (SHORT-NAME and SOFTWARE-COMPOSITION-TREF)</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that both composition-prototype are present in the produced output file</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide to the tool two ".dico" files, each one of them having the same SYSTEM-VERSION</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide to the tool two ".dico" files, each one of them having different SYSTEM-VERSION</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that only one label named SYSTEM-VERSION is present in the produced arxml file</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Check the tool behavior in case of arxml not well formed</t>
+  </si>
+  <si>
+    <t>Provide to the tool one ".arxml" file that is not correct (tags not properly closed, multiple roots, etc)</t>
+  </si>
+  <si>
+    <t>Check the tool behavior in case of dico not well formed</t>
+  </si>
+  <si>
+    <t>Provide to the tool one ".dico" file that is not correct (tags not properly closed, multiple roots, etc)</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>4/5/2018</t>
+  </si>
+  <si>
+    <t>- added new tests for other use-cases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -785,31 +1012,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -831,7 +1033,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1152,11 +1354,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1224,90 +1463,408 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1626,28 +2183,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="13" customWidth="1"/>
     <col min="3" max="3" width="68.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
@@ -1658,10 +2215,10 @@
         <v>12</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
@@ -1672,100 +2229,108 @@
         <v>16</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="15"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="15"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="14"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
       <c r="D10" s="14"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
       <c r="D11" s="14"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="14"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="14"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
       <c r="D14" s="14"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="14"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
@@ -1778,17 +2343,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" style="27" customWidth="1"/>
@@ -1798,7 +2363,7 @@
     <col min="6" max="6" width="10" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1818,17 +2383,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30.75" thickTop="1">
-      <c r="A2" s="33" t="s">
+    <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -1838,17 +2403,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="32" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -1858,17 +2423,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1878,17 +2443,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="34" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -1898,17 +2463,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="34" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -1918,13 +2483,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60">
-      <c r="A7" s="35"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="44" t="s">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="36" t="s">
         <v>46</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -1934,13 +2499,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45">
-      <c r="A8" s="35"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="44" t="s">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="34" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -1950,13 +2515,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="60">
-      <c r="A9" s="36"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="44" t="s">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="36" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="8" t="s">
@@ -1966,98 +2531,82 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C14" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D14" s="34" t="s">
         <v>8</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30">
-      <c r="A13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45">
-      <c r="A14" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="49" t="s">
-        <v>55</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>5</v>
@@ -2066,14 +2615,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45">
-      <c r="A15" s="36"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="49" t="s">
-        <v>59</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>8</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>5</v>
@@ -2082,35 +2635,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45">
-      <c r="A16" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="51" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="29"/>
-    </row>
-    <row r="17" spans="1:7" ht="45">
-      <c r="A17" s="35"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="49" t="s">
-        <v>65</v>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>52</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>5</v>
@@ -2119,31 +2675,34 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45">
-      <c r="A18" s="35"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="51" t="s">
-        <v>66</v>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="29"/>
-    </row>
-    <row r="19" spans="1:7" ht="60">
-      <c r="A19" s="35"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="49" t="s">
-        <v>67</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>59</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>5</v>
@@ -2152,14 +2711,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30">
-      <c r="A20" s="35"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="49" t="s">
-        <v>69</v>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>64</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>5</v>
@@ -2168,14 +2731,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="45">
-      <c r="A21" s="35"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="49" t="s">
-        <v>70</v>
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="49"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>65</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>5</v>
@@ -2184,14 +2747,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45">
-      <c r="A22" s="35"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>72</v>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>67</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>5</v>
@@ -2200,14 +2763,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="75">
-      <c r="A23" s="35"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="49" t="s">
-        <v>74</v>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="49"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>68</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>5</v>
@@ -2216,14 +2779,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30">
-      <c r="A24" s="35"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="49" t="s">
-        <v>91</v>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>70</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>5</v>
@@ -2232,14 +2795,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="60">
-      <c r="A25" s="36"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25" s="49" t="s">
-        <v>70</v>
+    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="49"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>72</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>5</v>
@@ -2248,18 +2811,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45">
-      <c r="A26" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="45" t="s">
-        <v>77</v>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="49"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>87</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>5</v>
@@ -2268,14 +2827,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30">
-      <c r="A27" s="36"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>81</v>
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="49"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>68</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>5</v>
@@ -2284,85 +2843,291 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="4" customFormat="1">
-      <c r="A28" s="23" t="s">
+    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="49"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="49"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="49"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="49"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="49"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="50"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="47"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B36" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="43"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="8" t="s">
+      <c r="D38" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F38" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30">
-      <c r="A29" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E29"/>
+  <autoFilter ref="A1:E37"/>
   <mergeCells count="10">
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="B16:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="A20:A33"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B20:B33"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E41:E1048576 E1:E38">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"not done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F38">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F38">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"not done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
@@ -2370,7 +3135,7 @@
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F30">
+  <conditionalFormatting sqref="F40">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
@@ -2378,16 +3143,16 @@
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F30">
+  <conditionalFormatting sqref="F40">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E40">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F40">
       <formula1>"YES, NO, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
DONE: added new tests to be implemented
</commit_message>
<xml_diff>
--- a/SystemDescriptor test plan.xlsx
+++ b/SystemDescriptor test plan.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000"/>
+    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="3" r:id="rId1"/>
     <sheet name="Overview" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Overview!$A$1:$E$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Overview!$A$1:$E$46</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="130">
   <si>
     <t>Requirements</t>
   </si>
@@ -85,12 +85,6 @@
     <t>TRS.SYSDESC.INOUT.001</t>
   </si>
   <si>
-    <t>not done</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>TRS.SYSDESC.INOUT.002</t>
   </si>
   <si>
@@ -974,9 +968,6 @@
     <t>- check that only one label named SYSTEM-VERSION is present in the produced arxml file</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Check the tool behavior in case of arxml not well formed</t>
   </si>
   <si>
@@ -996,6 +987,253 @@
   </si>
   <si>
     <t>- added new tests for other use-cases</t>
+  </si>
+  <si>
+    <t>TRS.SYSDESC.1</t>
+  </si>
+  <si>
+    <t>TRS.SYSDESC.2</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>5/2/2018</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- new test for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TRS.SYSDESC.FUNC.006</t>
+    </r>
+  </si>
+  <si>
+    <t>TRS.SYSDESC.FUNC.006</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: check that the tool will not generate the interfaces, types and all related data when the '-modularity' parameter is missing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: check that the tool generate the interfaces, types, and all related data when the '-modularity' parameter is given</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: check that the tool will not generate the COMPOSITION-SW-COMPONENT-TYPE component when the '-compo' parameter is missing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: check that the tool generate the COMPOSITION-SW-COMPONENT-TYPE component when the '-compo' parameter is given, followed by the correct composition SHORT-NAME</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: check that the tool will not generate the MAPPINGS component when the '-mapping' parameter is missing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: check that the tool generate the MAPPINGS component when the '-mapping' parameter is given, followed by the correct mappings SHORT-NAME</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: check that the tool will not generate the SYSTEM component when the '-system' parameter is missing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: check that the tool generate the SYSTEM component when the '-system' parameter is given, followed by the correct system SHORT-NAME</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: check that the tool does not execute when the '-config' parameter is missing</t>
+    </r>
+  </si>
+  <si>
+    <t>not done</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Check command-line arguments and their behaviour</t>
   </si>
 </sst>
 </file>
@@ -1019,18 +1257,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="31">
@@ -1395,7 +1627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1421,9 +1653,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1463,9 +1692,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1502,6 +1728,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1520,201 +1792,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2193,148 +2278,156 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="13" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="12" customWidth="1"/>
     <col min="3" max="3" width="68.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>83</v>
+      <c r="D1" s="27" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>84</v>
+      <c r="D2" s="15" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="61" t="s">
+      <c r="A3" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="14"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="14"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="14"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="14"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="14"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="14"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="14"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="14"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="13"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="14"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2344,268 +2437,268 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20:B33"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="79.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="79.140625" style="49" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="D3" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="E4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="B5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="B6" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="51"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="34" t="s">
+      <c r="C14" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="32" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="8" t="s">
@@ -2616,16 +2709,16 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>25</v>
+      <c r="A15" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="34" t="s">
+      <c r="C15" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="8" t="s">
@@ -2636,523 +2729,655 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>26</v>
+      <c r="A16" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="32"/>
+      <c r="E18" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="51"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="51"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="32"/>
+      <c r="E21" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="32"/>
+      <c r="E22" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="51"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="32"/>
+      <c r="E23" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="51"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="32"/>
+      <c r="E24" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="52"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="E26" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="61"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="51"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="51"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="51"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="51"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="51"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="51"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="51"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="51"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="51"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="51"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="51"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="51"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="52"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="61"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="37" t="s">
+      <c r="E45" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="57"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="43"/>
-      <c r="B38" s="45"/>
-      <c r="C38" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="57" t="s">
+      <c r="E48" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="C49" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="D39" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="B40" s="55" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>19</v>
+      <c r="D49" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E37"/>
-  <mergeCells count="10">
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
+  <autoFilter ref="A1:E46"/>
+  <mergeCells count="12">
     <mergeCell ref="A6:A13"/>
-    <mergeCell ref="A20:A33"/>
+    <mergeCell ref="A29:A42"/>
     <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B20:B33"/>
+    <mergeCell ref="B29:B42"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A17:A25"/>
+    <mergeCell ref="B17:B25"/>
   </mergeCells>
-  <conditionalFormatting sqref="E41:E1048576 E1:E38">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+  <conditionalFormatting sqref="E50:E1048576 E1:E47">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F38">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:F47">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F38">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+  <conditionalFormatting sqref="F2:F47">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+  <conditionalFormatting sqref="E48">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+  <conditionalFormatting sqref="F48">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+  <conditionalFormatting sqref="F48">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+  <conditionalFormatting sqref="E49">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="F49">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="F49">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E49">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F49">
       <formula1>"YES, NO, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
DONE: Tests after FUNC.006 implementation
</commit_message>
<xml_diff>
--- a/SystemDescriptor test plan.xlsx
+++ b/SystemDescriptor test plan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristi\PycharmProjects\SystemDescriptor\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
   </bookViews>
@@ -14,8 +19,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Overview!$A$1:$E$46</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1228,8 +1233,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1721,6 +1726,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1730,47 +1747,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2195,28 +2200,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="9" customWidth="1"/>
     <col min="3" max="3" width="68.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
@@ -2244,7 +2249,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>109</v>
       </c>
@@ -2258,7 +2263,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>114</v>
       </c>
@@ -2272,85 +2277,85 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
@@ -2363,31 +2368,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" style="58" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" style="45" customWidth="1"/>
     <col min="3" max="3" width="79.140625" style="41" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="38" t="s">
@@ -2403,7 +2408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30.75" thickTop="1">
+    <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>17</v>
       </c>
@@ -2423,7 +2428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
@@ -2443,7 +2448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>19</v>
       </c>
@@ -2463,7 +2468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>20</v>
       </c>
@@ -2483,8 +2488,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45">
-      <c r="A6" s="42" t="s">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="49" t="s">
@@ -2503,8 +2508,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60">
-      <c r="A7" s="43"/>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
       <c r="B7" s="50"/>
       <c r="C7" s="25" t="s">
         <v>51</v>
@@ -2519,8 +2524,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45">
-      <c r="A8" s="43"/>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
       <c r="B8" s="50"/>
       <c r="C8" s="25" t="s">
         <v>55</v>
@@ -2535,8 +2540,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60">
-      <c r="A9" s="43"/>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
       <c r="B9" s="50"/>
       <c r="C9" s="25" t="s">
         <v>56</v>
@@ -2551,8 +2556,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
-      <c r="A10" s="43"/>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
       <c r="B10" s="50"/>
       <c r="C10" s="27" t="s">
         <v>93</v>
@@ -2567,8 +2572,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30">
-      <c r="A11" s="43"/>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
       <c r="B11" s="50"/>
       <c r="C11" s="27" t="s">
         <v>94</v>
@@ -2583,8 +2588,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45">
-      <c r="A12" s="43"/>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
       <c r="B12" s="50"/>
       <c r="C12" s="25" t="s">
         <v>90</v>
@@ -2599,8 +2604,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30">
-      <c r="A13" s="44"/>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="48"/>
       <c r="B13" s="51"/>
       <c r="C13" s="27" t="s">
         <v>91</v>
@@ -2615,7 +2620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>22</v>
       </c>
@@ -2635,7 +2640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>23</v>
       </c>
@@ -2655,7 +2660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>24</v>
       </c>
@@ -2675,8 +2680,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="42" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
         <v>117</v>
       </c>
       <c r="B17" s="49" t="s">
@@ -2693,8 +2698,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30">
-      <c r="A18" s="43"/>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
       <c r="B18" s="50"/>
       <c r="C18" s="25" t="s">
         <v>125</v>
@@ -2707,8 +2712,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
-      <c r="A19" s="43"/>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
       <c r="B19" s="50"/>
       <c r="C19" s="27" t="s">
         <v>124</v>
@@ -2721,8 +2726,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30">
-      <c r="A20" s="43"/>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
       <c r="B20" s="50"/>
       <c r="C20" s="25" t="s">
         <v>123</v>
@@ -2735,8 +2740,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30">
-      <c r="A21" s="43"/>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="47"/>
       <c r="B21" s="50"/>
       <c r="C21" s="27" t="s">
         <v>122</v>
@@ -2749,8 +2754,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45">
-      <c r="A22" s="43"/>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
       <c r="B22" s="50"/>
       <c r="C22" s="25" t="s">
         <v>121</v>
@@ -2763,8 +2768,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30">
-      <c r="A23" s="43"/>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="47"/>
       <c r="B23" s="50"/>
       <c r="C23" s="25" t="s">
         <v>120</v>
@@ -2777,8 +2782,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30">
-      <c r="A24" s="43"/>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
       <c r="B24" s="50"/>
       <c r="C24" s="27" t="s">
         <v>119</v>
@@ -2791,8 +2796,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30">
-      <c r="A25" s="44"/>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="48"/>
       <c r="B25" s="51"/>
       <c r="C25" s="27" t="s">
         <v>118</v>
@@ -2805,7 +2810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>25</v>
       </c>
@@ -2825,8 +2830,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="45">
-      <c r="A27" s="45" t="s">
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="55" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="49" t="s">
@@ -2845,8 +2850,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45">
-      <c r="A28" s="47"/>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="58"/>
       <c r="B28" s="51"/>
       <c r="C28" s="29" t="s">
         <v>54</v>
@@ -2861,8 +2866,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="45">
-      <c r="A29" s="42" t="s">
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="46" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="52" t="s">
@@ -2881,8 +2886,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="60">
-      <c r="A30" s="43"/>
+    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
       <c r="B30" s="53"/>
       <c r="C30" s="29" t="s">
         <v>61</v>
@@ -2897,8 +2902,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30">
-      <c r="A31" s="43"/>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
       <c r="B31" s="53"/>
       <c r="C31" s="29" t="s">
         <v>64</v>
@@ -2913,8 +2918,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="45">
-      <c r="A32" s="43"/>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="47"/>
       <c r="B32" s="53"/>
       <c r="C32" s="29" t="s">
         <v>83</v>
@@ -2929,8 +2934,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="45">
-      <c r="A33" s="43"/>
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
       <c r="B33" s="53"/>
       <c r="C33" s="29" t="s">
         <v>67</v>
@@ -2945,8 +2950,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="75">
-      <c r="A34" s="43"/>
+    <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="47"/>
       <c r="B34" s="53"/>
       <c r="C34" s="29" t="s">
         <v>69</v>
@@ -2961,8 +2966,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30">
-      <c r="A35" s="43"/>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="47"/>
       <c r="B35" s="53"/>
       <c r="C35" s="29" t="s">
         <v>86</v>
@@ -2977,8 +2982,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="60">
-      <c r="A36" s="43"/>
+    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="47"/>
       <c r="B36" s="53"/>
       <c r="C36" s="29" t="s">
         <v>84</v>
@@ -2993,8 +2998,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="60">
-      <c r="A37" s="43"/>
+    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="47"/>
       <c r="B37" s="53"/>
       <c r="C37" s="29" t="s">
         <v>95</v>
@@ -3009,8 +3014,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="60">
-      <c r="A38" s="43"/>
+    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="47"/>
       <c r="B38" s="53"/>
       <c r="C38" s="29" t="s">
         <v>98</v>
@@ -3025,8 +3030,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30">
-      <c r="A39" s="43"/>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="47"/>
       <c r="B39" s="53"/>
       <c r="C39" s="29" t="s">
         <v>100</v>
@@ -3041,8 +3046,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="60">
-      <c r="A40" s="43"/>
+    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="47"/>
       <c r="B40" s="53"/>
       <c r="C40" s="29" t="s">
         <v>97</v>
@@ -3057,8 +3062,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30">
-      <c r="A41" s="43"/>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="47"/>
       <c r="B41" s="53"/>
       <c r="C41" s="29" t="s">
         <v>102</v>
@@ -3073,8 +3078,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30">
-      <c r="A42" s="44"/>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="48"/>
       <c r="B42" s="54"/>
       <c r="C42" s="29" t="s">
         <v>103</v>
@@ -3089,8 +3094,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="45">
-      <c r="A43" s="45" t="s">
+    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="55" t="s">
         <v>28</v>
       </c>
       <c r="B43" s="49" t="s">
@@ -3109,8 +3114,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30">
-      <c r="A44" s="47"/>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="58"/>
       <c r="B44" s="51"/>
       <c r="C44" s="25" t="s">
         <v>76</v>
@@ -3125,7 +3130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1">
+    <row r="45" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>29</v>
       </c>
@@ -3145,8 +3150,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30">
-      <c r="A46" s="45" t="s">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="55" t="s">
         <v>30</v>
       </c>
       <c r="B46" s="49" t="s">
@@ -3165,9 +3170,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A47" s="46"/>
-      <c r="B47" s="55"/>
+    <row r="47" spans="1:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="56"/>
+      <c r="B47" s="57"/>
       <c r="C47" s="32" t="s">
         <v>76</v>
       </c>
@@ -3181,11 +3186,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="43" t="s">
         <v>105</v>
       </c>
       <c r="C48" s="39" t="s">
@@ -3201,11 +3206,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="30.75" thickBot="1">
+    <row r="49" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="44" t="s">
         <v>107</v>
       </c>
       <c r="C49" s="40" t="s">

</xml_diff>

<commit_message>
New command-line New evolutions regarding the merge of DIAGNOSTIC-TABLE
</commit_message>
<xml_diff>
--- a/SystemDescriptor test plan.xlsx
+++ b/SystemDescriptor test plan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="137">
   <si>
     <t>Requirements</t>
   </si>
@@ -1228,6 +1228,114 @@
   </si>
   <si>
     <t>Check command-line arguments and their behaviour</t>
+  </si>
+  <si>
+    <t>TRS.DIAGNOSTIC.MERGE</t>
+  </si>
+  <si>
+    <t>Check that the tool concatenates correctly diagnostic tables</t>
+  </si>
+  <si>
+    <t>-check that the output arxml file contains only one diagnostic table that gathers elements from both input diagnostic tables</t>
+  </si>
+  <si>
+    <t>-check that the output arxml file contains only one diagnostic table that has only the mapped elements</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> provide two diagnostic tables with the same SHORT-NAME, each table having each DID mapped</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide two diagnostic tables with the same SHORT-NAME, each table having some DIDs mapped, while other DIDs are unmapped</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide two diagnostic tables with the same SHORT-NAME, but having ECU-INSTANCE-REF different</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Case 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: provide two diagnostic tables with the same SHORT-NAME, but having PROTOCOL-KIND different</t>
+    </r>
+  </si>
+  <si>
+    <t>- check that the tool wil not produce the output file
+-check that the log will contain the corresponding error</t>
   </si>
 </sst>
 </file>
@@ -1251,15 +1359,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1617,11 +1731,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1708,9 +1906,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1720,9 +1915,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1732,12 +1924,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1776,12 +1980,98 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2369,20 +2659,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" style="45" customWidth="1"/>
-    <col min="3" max="3" width="79.140625" style="41" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" style="42" customWidth="1"/>
+    <col min="3" max="3" width="79.140625" style="39" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
@@ -2392,10 +2682,10 @@
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -2489,10 +2779,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="51" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -2509,8 +2799,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="25" t="s">
         <v>51</v>
       </c>
@@ -2525,8 +2815,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="50"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="25" t="s">
         <v>55</v>
       </c>
@@ -2541,8 +2831,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="25" t="s">
         <v>56</v>
       </c>
@@ -2557,8 +2847,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="27" t="s">
         <v>93</v>
       </c>
@@ -2573,8 +2863,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="27" t="s">
         <v>94</v>
       </c>
@@ -2589,8 +2879,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="25" t="s">
         <v>90</v>
       </c>
@@ -2605,8 +2895,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="51"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="27" t="s">
         <v>91</v>
       </c>
@@ -2681,10 +2971,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="51" t="s">
         <v>127</v>
       </c>
       <c r="C17" s="27" t="s">
@@ -2699,8 +2989,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="50"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="25" t="s">
         <v>125</v>
       </c>
@@ -2713,8 +3003,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="27" t="s">
         <v>124</v>
       </c>
@@ -2727,8 +3017,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="25" t="s">
         <v>123</v>
       </c>
@@ -2741,8 +3031,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="27" t="s">
         <v>122</v>
       </c>
@@ -2755,8 +3045,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="52"/>
       <c r="C22" s="25" t="s">
         <v>121</v>
       </c>
@@ -2769,8 +3059,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="25" t="s">
         <v>120</v>
       </c>
@@ -2783,8 +3073,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="52"/>
       <c r="C24" s="27" t="s">
         <v>119</v>
       </c>
@@ -2797,8 +3087,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
-      <c r="B25" s="51"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="27" t="s">
         <v>118</v>
       </c>
@@ -2831,10 +3121,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="51" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="29" t="s">
@@ -2851,8 +3141,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="58"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="60"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="29" t="s">
         <v>54</v>
       </c>
@@ -2867,10 +3157,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="54" t="s">
         <v>59</v>
       </c>
       <c r="C29" s="29" t="s">
@@ -2887,8 +3177,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="53"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="29" t="s">
         <v>61</v>
       </c>
@@ -2903,8 +3193,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
-      <c r="B31" s="53"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="29" t="s">
         <v>64</v>
       </c>
@@ -2919,8 +3209,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="53"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="29" t="s">
         <v>83</v>
       </c>
@@ -2935,8 +3225,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="53"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="29" t="s">
         <v>67</v>
       </c>
@@ -2951,8 +3241,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
-      <c r="B34" s="53"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="29" t="s">
         <v>69</v>
       </c>
@@ -2967,8 +3257,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="53"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="29" t="s">
         <v>86</v>
       </c>
@@ -2983,8 +3273,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="53"/>
+      <c r="A36" s="49"/>
+      <c r="B36" s="55"/>
       <c r="C36" s="29" t="s">
         <v>84</v>
       </c>
@@ -2999,8 +3289,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
-      <c r="B37" s="53"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="55"/>
       <c r="C37" s="29" t="s">
         <v>95</v>
       </c>
@@ -3015,8 +3305,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
-      <c r="B38" s="53"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="55"/>
       <c r="C38" s="29" t="s">
         <v>98</v>
       </c>
@@ -3031,8 +3321,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
-      <c r="B39" s="53"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="29" t="s">
         <v>100</v>
       </c>
@@ -3047,8 +3337,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
-      <c r="B40" s="53"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="29" t="s">
         <v>97</v>
       </c>
@@ -3063,42 +3353,42 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="29" t="s">
+      <c r="A41" s="49"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="E41" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="6" t="s">
+      <c r="E41" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="47" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="48"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="29" t="s">
+      <c r="A42" s="50"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="6" t="s">
+      <c r="E42" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="47" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="51" t="s">
         <v>71</v>
       </c>
       <c r="C43" s="25" t="s">
@@ -3115,8 +3405,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="58"/>
-      <c r="B44" s="51"/>
+      <c r="A44" s="60"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="25" t="s">
         <v>76</v>
       </c>
@@ -3151,10 +3441,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="55" t="s">
+      <c r="A46" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="51" t="s">
         <v>75</v>
       </c>
       <c r="C46" s="25" t="s">
@@ -3171,8 +3461,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="56"/>
-      <c r="B47" s="57"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="59"/>
       <c r="C47" s="32" t="s">
         <v>76</v>
       </c>
@@ -3187,13 +3477,13 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="38" t="s">
         <v>106</v>
       </c>
       <c r="D48" s="34" t="s">
@@ -3207,28 +3497,98 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="44" t="s">
+      <c r="B49" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="C49" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="33" t="s">
+      <c r="D49" s="28" t="s">
         <v>66</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F49" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="71"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="71"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D52" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="72"/>
+      <c r="B53" s="66"/>
+      <c r="C53" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E46"/>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="A50:A53"/>
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="A29:A42"/>
     <mergeCell ref="B6:B13"/>
@@ -3242,74 +3602,74 @@
     <mergeCell ref="A17:A25"/>
     <mergeCell ref="B17:B25"/>
   </mergeCells>
-  <conditionalFormatting sqref="E50:E1048576 E1:E47">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+  <conditionalFormatting sqref="E54:E1048576 E1:E47">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F47">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F47">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+  <conditionalFormatting sqref="E49:E53">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="F49:F53">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="F49:F53">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E53">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F53">
       <formula1>"YES, NO, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>